<commit_message>
week13. discuss with teacher
</commit_message>
<xml_diff>
--- a/doc/res.xlsx
+++ b/doc/res.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
   <si>
     <t>thr</t>
   </si>
@@ -28,6 +28,9 @@
     <t>crb</t>
   </si>
   <si>
+    <t>cpr</t>
+  </si>
+  <si>
     <t>got</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
   </si>
   <si>
     <t>libc-jop</t>
-  </si>
-  <si>
-    <t>fsb-vtb</t>
   </si>
 </sst>
 </file>
@@ -72,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -116,8 +116,97 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,16 +220,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,75 +230,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,20 +243,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -271,13 +271,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,169 +439,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,39 +476,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,6 +510,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -560,11 +538,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,144 +553,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -727,7 +727,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -762,6 +762,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,18 +1091,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="252" zoomScaleNormal="252" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="9.9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1113,208 +1116,239 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1"/>
       <c r="B11" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>